<commit_message>
full elec and industry files from RMI
</commit_message>
<xml_diff>
--- a/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
+++ b/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
@@ -697,7 +697,7 @@
           <t>Source:</t>
         </is>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>Energy Information Administration</t>
         </is>
@@ -759,7 +759,7 @@
     </row>
     <row r="11" ht="14.25" customHeight="1" s="30">
       <c r="A11" s="12" t="n"/>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>EIA form 860 3_1_Generator_Y2018.xlsx</t>
         </is>
@@ -823,7 +823,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1" s="30">
       <c r="A13" s="12" t="n"/>
-      <c r="B13" s="6" t="inlineStr">
+      <c r="B13" s="7" t="inlineStr">
         <is>
           <t>3_1_Generator_Y2018.xlsx "Operable"</t>
         </is>

</xml_diff>